<commit_message>
Updated css and machineview
</commit_message>
<xml_diff>
--- a/img/tables.xlsx
+++ b/img/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Web developer\Projects\iubh_dashboard\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2265D12-A3ED-46B0-8428-049D2C817400}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C102751F-13FF-4F2D-B921-0AF19E15555E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{B5D08A16-A98F-47A7-93AC-FA06C72F0F2C}"/>
   </bookViews>
@@ -118,12 +118,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -132,13 +129,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Zeit</a:t>
+              <a:t>Zeit / Temperatur</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> / Temperatur</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -155,12 +147,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -181,26 +170,33 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="28575" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:alpha val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -841,6 +837,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="lt1">
+                      <a:alpha val="0"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
         <c:smooth val="0"/>
         <c:axId val="1048393167"/>
         <c:axId val="1048086735"/>
@@ -858,12 +875,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="lt1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -874,12 +888,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -903,20 +914,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="0\ &quot;°C&quot;" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -935,10 +932,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -966,14 +960,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="accent1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1018,12 +1009,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1050,12 +1038,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1076,26 +1061,33 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent1"/>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="28575" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent2">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                    <a:alpha val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1736,6 +1728,27 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1"/>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="lt1">
+                      <a:alpha val="0"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
         <c:smooth val="0"/>
         <c:axId val="1080820351"/>
         <c:axId val="1044595039"/>
@@ -1753,12 +1766,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:schemeClr val="lt1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1769,12 +1779,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1798,20 +1805,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="_([$EUR]\ * #,##0.00_);_([$EUR]\ * \(#,##0.00\);_([$EUR]\ * &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1830,10 +1823,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1861,14 +1851,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="accent1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1973,59 +1960,53 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="229">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="100" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -2037,22 +2018,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2060,10 +2037,7 @@
       </a:solidFill>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -2074,71 +2048,87 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="22225">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -2147,10 +2137,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2162,31 +2152,30 @@
     </cs:spPr>
   </cs:dataPointWireframe>
   <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2195,15 +2184,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2214,37 +2203,51 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
   <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:errorBar>
   <cs:floor>
@@ -2252,28 +2255,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2281,165 +2279,174 @@
     </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
   </cs:trendline>
   <cs:trendlineLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2447,13 +2454,15 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2464,10 +2473,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -2476,72 +2482,60 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="229">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" spc="100" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -2553,22 +2547,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2576,10 +2566,7 @@
       </a:solidFill>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -2590,71 +2577,87 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:pattFill prst="ltUpDiag">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="22225">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -2663,10 +2666,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2678,31 +2681,30 @@
     </cs:spPr>
   </cs:dataPointWireframe>
   <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2711,15 +2713,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2730,37 +2732,51 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:alpha val="0"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
   <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:errorBar>
   <cs:floor>
@@ -2768,28 +2784,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2797,165 +2808,174 @@
     </cs:spPr>
   </cs:gridlineMajor>
   <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
   </cs:trendline>
   <cs:trendlineLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -2963,13 +2983,15 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2980,10 +3002,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -2992,14 +3011,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3380,8 +3393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F634563D-3F0B-42A4-92A1-11D0E8695B49}">
   <dimension ref="B3:R103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S5" zoomScale="171" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="141" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>